<commit_message>
fix data and script
</commit_message>
<xml_diff>
--- a/17.12.21_MTS_PC3/PC3_results/PC3.xlsx
+++ b/17.12.21_MTS_PC3/PC3_results/PC3.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -455,60 +455,80 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>CC50</t>
+          <t>CC50.x</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>CC50.y</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Lower</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Upper</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>SE</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>OA</t>
+          <t>DMSO</t>
         </is>
       </c>
       <c r="B2">
-        <v>4.068</v>
+        <v>0.546</v>
       </c>
       <c r="C2">
-        <v>0.02</v>
+        <v>0.705</v>
       </c>
       <c r="D2">
-        <v>5.78</v>
+        <v>-3.491</v>
       </c>
       <c r="E2">
-        <v>83.95399999999999</v>
+        <v>71.675</v>
       </c>
       <c r="F2">
-        <v>134.049</v>
+        <v>100.052</v>
       </c>
       <c r="G2">
-        <v>9.542999999999999</v>
+        <v>0.151</v>
       </c>
       <c r="H2">
-        <v>11.155</v>
+        <v>9.481999999999999</v>
       </c>
       <c r="I2">
-        <v>11.1</v>
+        <v>12.97</v>
       </c>
       <c r="J2">
-        <v>7.259</v>
+        <v>4.926</v>
       </c>
       <c r="K2">
-        <v>3.536</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="L2">
-        <v>0.518</v>
+        <v>-0.368</v>
       </c>
       <c r="M2">
-        <v>7.564</v>
+        <v>5.526</v>
       </c>
       <c r="N2">
-        <v>18.467</v>
+        <v>20.309</v>
       </c>
       <c r="O2">
-        <v>2.699</v>
+        <v>1.783</v>
       </c>
       <c r="P2">
-        <v>0.61</v>
+        <v>0.717</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -517,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0.014</v>
+        <v>0.091</v>
       </c>
       <c r="T2">
         <v>100</v>
@@ -526,56 +546,153 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>MMAE</t>
         </is>
       </c>
       <c r="B3">
-        <v>6.48</v>
+        <v>1.191</v>
       </c>
       <c r="C3">
-        <v>0.003</v>
+        <v>0.355</v>
       </c>
       <c r="D3">
-        <v>-0.02</v>
+        <v>1.194</v>
       </c>
       <c r="E3">
-        <v>51.541</v>
+        <v>28.102</v>
       </c>
       <c r="F3">
-        <v>191.672</v>
+        <v>63.048</v>
       </c>
       <c r="G3">
-        <v>4524.052</v>
+        <v>0.001</v>
       </c>
       <c r="H3">
-        <v>0.33</v>
+        <v>1.186</v>
       </c>
       <c r="I3">
-        <v>1236.227</v>
+        <v>4.984</v>
       </c>
       <c r="J3">
-        <v>1197.465</v>
+        <v>4.354</v>
+      </c>
+      <c r="K3">
+        <v>0.001</v>
       </c>
       <c r="L3">
-        <v>-0.06</v>
+        <v>1.007</v>
       </c>
       <c r="M3">
-        <v>0.042</v>
+        <v>5.639</v>
       </c>
       <c r="N3">
-        <v>0.16</v>
+        <v>14.48</v>
+      </c>
+      <c r="O3">
+        <v>1.262</v>
       </c>
       <c r="P3">
-        <v>0.953</v>
+        <v>0.327</v>
       </c>
       <c r="Q3">
-        <v>0.967</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>0.875</v>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0.222</v>
       </c>
       <c r="T3">
-        <v>100</v>
+        <v>2.753623717932641e-012</v>
+      </c>
+      <c r="U3">
+        <v>0.001661953671243145</v>
+      </c>
+      <c r="V3">
+        <v>-0.002253639655625769</v>
+      </c>
+      <c r="W3">
+        <v>0.005577546998112059</v>
+      </c>
+      <c r="X3">
+        <v>0.0014102902015021</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MMP62</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>1.342</v>
+      </c>
+      <c r="C4">
+        <v>0.3</v>
+      </c>
+      <c r="D4">
+        <v>1.441</v>
+      </c>
+      <c r="E4">
+        <v>24.495</v>
+      </c>
+      <c r="F4">
+        <v>78.867</v>
+      </c>
+      <c r="G4">
+        <v>0.332</v>
+      </c>
+      <c r="H4">
+        <v>0.481</v>
+      </c>
+      <c r="I4">
+        <v>3.613</v>
+      </c>
+      <c r="J4">
+        <v>3.566</v>
+      </c>
+      <c r="K4">
+        <v>0.117</v>
+      </c>
+      <c r="L4">
+        <v>2.996</v>
+      </c>
+      <c r="M4">
+        <v>6.78</v>
+      </c>
+      <c r="N4">
+        <v>22.114</v>
+      </c>
+      <c r="O4">
+        <v>2.84</v>
+      </c>
+      <c r="P4">
+        <v>0.007</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0.01</v>
+      </c>
+      <c r="T4">
+        <v>0.3600000000027537</v>
+      </c>
+      <c r="U4">
+        <v>0.4719423107703062</v>
+      </c>
+      <c r="V4">
+        <v>0.3025823117782635</v>
+      </c>
+      <c r="W4">
+        <v>0.6413023097623489</v>
+      </c>
+      <c r="X4">
+        <v>0.06099886458226141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>